<commit_message>
Sonar lint code smell
</commit_message>
<xml_diff>
--- a/03_PizzaShop/Docs/initial/Lab01_ReviewReport.xlsx
+++ b/03_PizzaShop/Docs/initial/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scoala\Laborator\Anul_3\Semestrul_2\VVSSPizzaShop\03_PizzaShop\Docs\initial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889610C8-526B-453E-8356-17999E62534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831B88E-B841-4518-8FD3-1FA6EFA20136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -200,9 +200,6 @@
   </si>
   <si>
     <t>MenuRepository/33</t>
-  </si>
-  <si>
-    <t>SonarLint: Combine with this catch</t>
   </si>
   <si>
     <t>catch (FileNotFoundException e) {
@@ -234,18 +231,255 @@
   <si>
     <t>No package distribution in the diagram</t>
   </si>
+  <si>
+    <t>Combine with this catch</t>
+  </si>
+  <si>
+    <t>DataService/36</t>
+  </si>
+  <si>
+    <t>Collection.isEmpty() should be used to test for emptiness</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>) ||(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>.size()==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF1750EB"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">)) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>total;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>((</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>==</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>null</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>) ||(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF000000"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>l</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">.isEmpty())) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF0033B3"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">return </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.8000000000000007"/>
+        <color rgb="FF080808"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t>total;</t>
+    </r>
+  </si>
+  <si>
+    <t>MenuRepository/24</t>
+  </si>
+  <si>
+    <t>Resources should be closed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+        try {
+            br = new BufferedReader(new FileReader(file));
+            String line = null;
+            while((line=br.readLine())!=null){
+                MenuDataModel menuItem=getMenuItem(line);
+                listMenu.add(menuItem);
+            }
+            br.close();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        try(BufferedReader br = new BufferedReader(new FileReader(file))){
+            String line = null;
+            while((line=br.readLine())!=null){
+                MenuDataModel menuItem=getMenuItem(line);
+                listMenu.add(menuItem);
+            }
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -323,6 +557,30 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF080808"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF0033B3"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF000000"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF1750EB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="5">
@@ -424,82 +682,86 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -849,7 +1111,7 @@
       <selection activeCell="D7" sqref="D7:E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
@@ -861,24 +1123,24 @@
     <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -887,7 +1149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -898,14 +1160,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="28"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -916,14 +1178,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="30"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -934,26 +1196,26 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="24">
         <v>44631</v>
       </c>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -967,7 +1229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -975,7 +1237,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -984,7 +1246,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -993,7 +1255,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1002,7 +1264,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1011,7 +1273,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1020,7 +1282,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1029,7 +1291,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1038,7 +1300,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1047,7 +1309,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1056,7 +1318,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1065,7 +1327,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1074,7 +1336,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1083,7 +1345,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="16"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1092,7 +1354,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="16"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1101,7 +1363,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="16"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1110,10 +1372,10 @@
       <c r="D25" s="3"/>
       <c r="E25" s="16"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="E26" s="11"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="C27" s="12" t="s">
         <v>8</v>
       </c>
@@ -1141,11 +1403,11 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
@@ -1156,24 +1418,24 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1182,7 +1444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1193,14 +1455,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="31"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1211,14 +1473,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="33"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1229,26 +1491,26 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="24">
         <v>44631</v>
       </c>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1262,45 +1524,45 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>58</v>
+      <c r="C10" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E10" s="23" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>59</v>
+      <c r="C11" s="23" t="s">
+        <v>58</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E11" s="23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="38" t="s">
-        <v>60</v>
+      <c r="C12" s="23" t="s">
+        <v>59</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="38" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E12" s="23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1309,7 +1571,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1318,7 +1580,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1327,7 +1589,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1336,7 +1598,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1345,7 +1607,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1354,7 +1616,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1363,7 +1625,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1372,7 +1634,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1381,7 +1643,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1390,7 +1652,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1399,7 +1661,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1408,7 +1670,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1417,7 +1679,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1426,10 +1688,10 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="C28" s="12" t="s">
         <v>8</v>
       </c>
@@ -1458,10 +1720,10 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
@@ -1473,24 +1735,24 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1499,7 +1761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1510,14 +1772,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1528,14 +1790,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="35"/>
+      <c r="E5" s="36"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1546,26 +1808,26 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="24"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E6" s="25"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="24">
         <v>44631</v>
       </c>
-      <c r="E7" s="24"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E7" s="25"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1593,7 +1855,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.8">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1608,7 +1870,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="28.8">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -1623,7 +1885,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="28.8">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1638,7 +1900,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1647,7 +1909,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1656,7 +1918,7 @@
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1665,7 +1927,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1674,7 +1936,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1683,7 +1945,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1692,7 +1954,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1701,7 +1963,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1710,7 +1972,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1719,7 +1981,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1728,7 +1990,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1737,7 +1999,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1746,7 +2008,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1755,7 +2017,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1764,7 +2026,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1773,7 +2035,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1782,7 +2044,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1791,10 +2053,10 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5">
       <c r="C32" s="12" t="s">
         <v>8</v>
       </c>
@@ -1822,41 +2084,41 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
     <col min="3" max="3" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.88671875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="54.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="52.5546875" style="6" customWidth="1"/>
     <col min="7" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="26.77734375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="25" t="s">
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="B2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1865,7 +2127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
@@ -1876,14 +2138,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="33"/>
+      <c r="E4" s="34"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1894,14 +2156,14 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="24"/>
+      <c r="E5" s="25"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1912,18 +2174,23 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="24">
         <v>44631</v>
       </c>
-      <c r="E6" s="24"/>
+      <c r="E6" s="25"/>
       <c r="F6" s="21"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
+      <c r="D7" s="40" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -1940,7 +2207,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -1957,7 +2224,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="72">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -1966,36 +2233,52 @@
         <v>54</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="39" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="172.8">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2005,7 +2288,7 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2015,7 +2298,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2025,7 +2308,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2035,7 +2318,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2045,7 +2328,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2055,7 +2338,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2065,7 +2348,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2075,7 +2358,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2085,7 +2368,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2095,7 +2378,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2105,7 +2388,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2115,7 +2398,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2125,7 +2408,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2135,7 +2418,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2145,7 +2428,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2155,7 +2438,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2165,15 +2448,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6">
       <c r="E31" s="11"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C32" s="36" t="s">
+    <row r="32" spans="2:6">
+      <c r="C32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="38"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed some warnings using SonarLint
</commit_message>
<xml_diff>
--- a/03_PizzaShop/Docs/initial/Lab01_ReviewReport.xlsx
+++ b/03_PizzaShop/Docs/initial/Lab01_ReviewReport.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Scoala\Laborator\Anul_3\Semestrul_2\VVSSPizzaShop\03_PizzaShop\Docs\initial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Info\Lab1-Git\VVSSPizzaShop\03_PizzaShop\Docs\initial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7831B88E-B841-4518-8FD3-1FA6EFA20136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0D6F20-ACDF-46B9-A344-31B7B493085B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -460,6 +460,49 @@
         } catch (IOException e) {
             e.printStackTrace();
         }</t>
+  </si>
+  <si>
+    <t>try {
+            br = new BufferedReader(new FileReader(file));
+            String line = null;
+            while((line=br.readLine())!=null){
+                Payment payment=getPayment(line);
+                paymentList.add(payment);
+            }
+            br.close();
+        } catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>PaymentRepository/26</t>
+  </si>
+  <si>
+    <t>try (BufferedReader br = new BufferedReader(new FileReader(file))){
+            String line = null;
+            while((line=br.readLine())!=null){
+                Payment payment=getPayment(line);
+                paymentList.add(payment);
+            }
+        } catch (FileNotFoundException e) {
+            e.printStackTrace();
+        } catch (IOException e) {
+            e.printStackTrace();
+        }</t>
+  </si>
+  <si>
+    <t>KitchenGUIController/23</t>
+  </si>
+  <si>
+    <t>Constructors should not be used to instantiate "String", "BigInteger", "BigDecimal" and primitive-wrapper classes</t>
+  </si>
+  <si>
+    <t>private String extractedTableNumberString = new String();</t>
+  </si>
+  <si>
+    <t>private String extractedTableNumberString;</t>
   </si>
 </sst>
 </file>
@@ -715,6 +758,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -760,10 +807,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1128,19 +1171,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1164,10 +1207,10 @@
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="28"/>
+      <c r="E4" s="30"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1182,10 +1225,10 @@
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="30"/>
+      <c r="E5" s="32"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1201,19 +1244,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="26">
         <v>44631</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1423,19 +1466,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1459,10 +1502,10 @@
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31"/>
+      <c r="E4" s="33"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1477,10 +1520,10 @@
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="32" t="s">
+      <c r="D5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="35"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1496,19 +1539,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="26">
         <v>44631</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -1740,19 +1783,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -1776,10 +1819,10 @@
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1794,10 +1837,10 @@
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="36"/>
+      <c r="E5" s="38"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1813,19 +1856,19 @@
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="26">
         <v>44631</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="27"/>
     </row>
     <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
@@ -2084,7 +2127,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -2092,7 +2135,7 @@
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.21875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.21875" style="6" customWidth="1"/>
     <col min="4" max="4" width="32.88671875" style="6" customWidth="1"/>
     <col min="5" max="5" width="54.6640625" style="6" customWidth="1"/>
     <col min="6" max="6" width="52.5546875" style="6" customWidth="1"/>
@@ -2106,19 +2149,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>30</v>
@@ -2142,10 +2185,10 @@
       <c r="C4" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="36"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -2160,10 +2203,10 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="27"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -2179,14 +2222,14 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="24">
+      <c r="D6" s="26">
         <v>44631</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="27"/>
       <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="D7" s="40" t="s">
+      <c r="D7" s="25" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2253,10 +2296,10 @@
       <c r="D12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="39" t="s">
+      <c r="F12" s="24" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2278,25 +2321,41 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" ht="187.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="C14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.4" customHeight="1">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="C15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="B16" s="3">
@@ -2452,11 +2511,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6">
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
+      <c r="D32" s="40"/>
+      <c r="E32" s="40"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Requirements_v2.0.pdf and modified Lab01_ReviewReport.xlsx
</commit_message>
<xml_diff>
--- a/03_PizzaShop/Docs/initial/Lab01_ReviewReport.xlsx
+++ b/03_PizzaShop/Docs/initial/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Info\Lab1-Git\VVSSPizzaShop\03_PizzaShop\Docs\initial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0D6F20-ACDF-46B9-A344-31B7B493085B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FC8809-7CA8-4AF4-A331-FB8C7B579F20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -503,6 +503,24 @@
   </si>
   <si>
     <t>private String extractedTableNumberString;</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>R04</t>
+  </si>
+  <si>
+    <t>All the major requirements are missing</t>
+  </si>
+  <si>
+    <t>Pizza types and prices aren't specified</t>
+  </si>
+  <si>
+    <t>The actual payment is missing in F01</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1168,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1276,27 +1294,39 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>79</v>
+      </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="B13" s="3">
@@ -2127,7 +2157,7 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>

</xml_diff>